<commit_message>
[LP-26378207] rearrange columns again
</commit_message>
<xml_diff>
--- a/reconstruction_verification/static/template.xlsx
+++ b/reconstruction_verification/static/template.xlsx
@@ -6,7 +6,7 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Catch Data" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -17,24 +17,72 @@
     <t>fishing entity</t>
   </si>
   <si>
-    <t xml:space="preserve">original country fishing </t>
-  </si>
-  <si>
     <t>EEZ</t>
   </si>
   <si>
+    <t>FAO area</t>
+  </si>
+  <si>
+    <t>layer</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t>catch type</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>taxon name</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>input type</t>
+  </si>
+  <si>
+    <t>original country fishing</t>
+  </si>
+  <si>
     <t>EEZ sub area</t>
   </si>
   <si>
-    <t>FAO area</t>
-  </si>
-  <si>
     <t>subregional area</t>
   </si>
   <si>
     <t>province state</t>
   </si>
   <si>
+    <t>original sector</t>
+  </si>
+  <si>
+    <t>original taxon name</t>
+  </si>
+  <si>
+    <t>original FAO name</t>
+  </si>
+  <si>
+    <t>adjustment factor</t>
+  </si>
+  <si>
+    <t>gear type</t>
+  </si>
+  <si>
+    <t>forward carry rule</t>
+  </si>
+  <si>
+    <t>disaggregation rule</t>
+  </si>
+  <si>
+    <t>layer rule</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
     <t>ICES area</t>
   </si>
   <si>
@@ -42,54 +90,6 @@
   </si>
   <si>
     <t>CCAMLR area</t>
-  </si>
-  <si>
-    <t>layer</t>
-  </si>
-  <si>
-    <t>sector</t>
-  </si>
-  <si>
-    <t>original sector</t>
-  </si>
-  <si>
-    <t>catch type</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>taxon name</t>
-  </si>
-  <si>
-    <t>original taxon name</t>
-  </si>
-  <si>
-    <t>original FAO name</t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>adjustment factor</t>
-  </si>
-  <si>
-    <t>gear type</t>
-  </si>
-  <si>
-    <t>input type</t>
-  </si>
-  <si>
-    <t>forward carry rule</t>
-  </si>
-  <si>
-    <t>disaggregation rule</t>
-  </si>
-  <si>
-    <t>layer rule</t>
-  </si>
-  <si>
-    <t>notes</t>
   </si>
 </sst>
 </file>
@@ -99,7 +99,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -111,53 +111,25 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Courier New"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="11"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -167,53 +139,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="9"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -223,27 +158,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -262,9 +188,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffb4c6e7"/>
       <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1496,400 +1420,372 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="9.125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9.125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="9.125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="9.125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="9.125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="9.125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="9.125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="9.125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9.125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="9.125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="9.125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="9.125" style="1" customWidth="1"/>
-    <col min="27" max="256" width="9" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6" style="1" customWidth="1"/>
+    <col min="8" max="8" width="6" style="1" customWidth="1"/>
+    <col min="9" max="9" width="6" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6" style="1" customWidth="1"/>
+    <col min="11" max="11" width="6" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6" style="1" customWidth="1"/>
+    <col min="14" max="14" width="6" style="1" customWidth="1"/>
+    <col min="15" max="15" width="6" style="1" customWidth="1"/>
+    <col min="16" max="16" width="6" style="1" customWidth="1"/>
+    <col min="17" max="17" width="6" style="1" customWidth="1"/>
+    <col min="18" max="18" width="6" style="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" customWidth="1"/>
+    <col min="20" max="20" width="6" style="1" customWidth="1"/>
+    <col min="21" max="21" width="6" style="1" customWidth="1"/>
+    <col min="22" max="22" width="6" style="1" customWidth="1"/>
+    <col min="23" max="23" width="6" style="1" customWidth="1"/>
+    <col min="24" max="24" width="6" style="1" customWidth="1"/>
+    <col min="25" max="25" width="6" style="1" customWidth="1"/>
+    <col min="26" max="26" width="6" style="1" customWidth="1"/>
+    <col min="27" max="256" width="6" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row r="1" ht="17" customHeight="1">
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="3">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" t="s" s="2">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="3">
+      <c r="F1" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="3">
+      <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="3">
+      <c r="H1" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="3">
+      <c r="I1" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="3">
+      <c r="J1" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="3">
+      <c r="K1" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="3">
+      <c r="L1" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="3">
+      <c r="M1" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="3">
+      <c r="N1" t="s" s="2">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="3">
+      <c r="O1" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="3">
+      <c r="P1" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="Q1" t="s" s="3">
+      <c r="Q1" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="R1" t="s" s="3">
+      <c r="R1" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="S1" t="s" s="3">
+      <c r="S1" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="T1" t="s" s="3">
+      <c r="T1" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="U1" t="s" s="3">
+      <c r="U1" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="V1" t="s" s="3">
+      <c r="V1" t="s" s="2">
         <v>21</v>
       </c>
-      <c r="W1" t="s" s="3">
+      <c r="W1" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="X1" t="s" s="3">
+      <c r="X1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="Y1" t="s" s="3">
+      <c r="Y1" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="Z1" t="s" s="4">
+      <c r="Z1" t="s" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="2" ht="20.35" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
+    <row r="2" ht="17" customHeight="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
     </row>
-    <row r="3" ht="20.35" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
+    <row r="3" ht="17" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
     </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
+    <row r="4" ht="17" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
     </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
+    <row r="5" ht="17" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
     </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
+    <row r="6" ht="17" customHeight="1">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
     </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
+    <row r="7" ht="17" customHeight="1">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
     </row>
-    <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
+    <row r="8" ht="17" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
     </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
+    <row r="9" ht="17" customHeight="1">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
     </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-      <c r="U10" s="6"/>
-      <c r="V10" s="6"/>
-      <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
+    <row r="10" ht="17" customHeight="1">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated to add the taxon_notes column to the raw_catch table and to adjust the model to match with the new reference table.
</commit_message>
<xml_diff>
--- a/reconstruction_verification/static/template.xlsx
+++ b/reconstruction_verification/static/template.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeaAroundUs\recon-verification\reconstruction_verification\static\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>fishing entity</t>
   </si>
@@ -90,33 +97,23 @@
   </si>
   <si>
     <t>CCAMLR area</t>
+  </si>
+  <si>
+    <t>taxon notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="13"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
@@ -154,23 +151,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -179,23 +172,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -387,7 +442,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -396,7 +451,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -405,7 +460,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -414,7 +469,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -423,7 +478,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -432,7 +487,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -544,8 +599,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -553,14 +608,14 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -579,7 +634,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -587,7 +642,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -615,7 +670,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -641,7 +696,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -667,7 +722,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -693,7 +748,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -719,7 +774,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -745,7 +800,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -771,7 +826,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -797,7 +852,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -823,7 +878,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -836,9 +891,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -854,7 +915,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -873,7 +934,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -899,7 +960,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -925,7 +986,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -951,7 +1012,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -977,7 +1038,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1003,7 +1064,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1029,7 +1090,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1055,7 +1116,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1081,7 +1142,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1107,7 +1168,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1120,9 +1181,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1135,7 +1202,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1154,7 +1221,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1184,7 +1251,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1210,7 +1277,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1236,7 +1303,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1262,7 +1329,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1288,7 +1355,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1314,7 +1381,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1340,7 +1407,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1366,7 +1433,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1392,7 +1459,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1405,137 +1472,125 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AB1" sqref="AB1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6" style="1" customWidth="1"/>
-    <col min="4" max="4" width="6" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6" style="1" customWidth="1"/>
-    <col min="14" max="14" width="6" style="1" customWidth="1"/>
-    <col min="15" max="15" width="6" style="1" customWidth="1"/>
-    <col min="16" max="16" width="6" style="1" customWidth="1"/>
-    <col min="17" max="17" width="6" style="1" customWidth="1"/>
-    <col min="18" max="18" width="6" style="1" customWidth="1"/>
-    <col min="19" max="19" width="6" style="1" customWidth="1"/>
-    <col min="20" max="20" width="6" style="1" customWidth="1"/>
-    <col min="21" max="21" width="6" style="1" customWidth="1"/>
-    <col min="22" max="22" width="6" style="1" customWidth="1"/>
-    <col min="23" max="23" width="6" style="1" customWidth="1"/>
-    <col min="24" max="24" width="6" style="1" customWidth="1"/>
-    <col min="25" max="25" width="6" style="1" customWidth="1"/>
-    <col min="26" max="26" width="6" style="1" customWidth="1"/>
+    <col min="1" max="25" width="6" style="1" customWidth="1"/>
+    <col min="26" max="26" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="256" width="6" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="17" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="2">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="2">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="2">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="2">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="2">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="2">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s" s="2">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s" s="2">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s" s="2">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s" s="2">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s" s="2">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s" s="2">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s" s="2">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s" s="2">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s" s="2">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s" s="2">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" ht="17" customHeight="1">
+    <row r="2" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1562,8 +1617,9 @@
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
     </row>
-    <row r="3" ht="17" customHeight="1">
+    <row r="3" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1590,8 +1646,9 @@
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
     </row>
-    <row r="4" ht="17" customHeight="1">
+    <row r="4" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1618,8 +1675,9 @@
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
     </row>
-    <row r="5" ht="17" customHeight="1">
+    <row r="5" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1646,8 +1704,9 @@
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
     </row>
-    <row r="6" ht="17" customHeight="1">
+    <row r="6" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1674,8 +1733,9 @@
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
     </row>
-    <row r="7" ht="17" customHeight="1">
+    <row r="7" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1702,8 +1762,9 @@
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
     </row>
-    <row r="8" ht="17" customHeight="1">
+    <row r="8" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1730,8 +1791,9 @@
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
     </row>
-    <row r="9" ht="17" customHeight="1">
+    <row r="9" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1758,8 +1820,9 @@
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
     </row>
-    <row r="10" ht="17" customHeight="1">
+    <row r="10" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1786,10 +1849,11 @@
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Modified as part of the effort to split catch_type and introduce reporting_status.
</commit_message>
<xml_diff>
--- a/reconstruction_verification/static/template.xlsx
+++ b/reconstruction_verification/static/template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>fishing entity</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>taxon notes</t>
+  </si>
+  <si>
+    <t>reporting status</t>
   </si>
 </sst>
 </file>
@@ -1494,20 +1497,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV10"/>
+  <dimension ref="A1:IW10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="25" width="6" style="1" customWidth="1"/>
-    <col min="26" max="26" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="256" width="6" style="1" customWidth="1"/>
+    <col min="1" max="5" width="6" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.19921875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="26" width="6" style="1" customWidth="1"/>
+    <col min="27" max="27" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="257" width="6" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1527,70 +1533,73 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1618,8 +1627,9 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
       <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
     </row>
-    <row r="3" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1647,8 +1657,9 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
     </row>
-    <row r="4" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -1676,8 +1687,9 @@
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
     </row>
-    <row r="5" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -1705,8 +1717,9 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
     </row>
-    <row r="6" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -1734,8 +1747,9 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
     </row>
-    <row r="7" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1763,8 +1777,9 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
     </row>
-    <row r="8" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1792,8 +1807,9 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
     </row>
-    <row r="9" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1821,8 +1837,9 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
     </row>
-    <row r="10" spans="1:27" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1850,6 +1867,7 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Template modified to accommodate gear notes column.
</commit_message>
<xml_diff>
--- a/reconstruction_verification/static/template.xlsx
+++ b/reconstruction_verification/static/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeaAroundUs\recon-verification\reconstruction_verification\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.sy\Documents\GitHub\recon-verification\reconstruction_verification\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1500,7 +1500,7 @@
   <dimension ref="A1:IW10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="M1" sqref="M1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="12.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1508,9 +1508,9 @@
     <col min="1" max="5" width="6" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.19921875" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="26" width="6" style="1" customWidth="1"/>
-    <col min="27" max="27" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="257" width="6" style="1" customWidth="1"/>
+    <col min="8" max="14" width="6" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="257" width="6" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -1548,52 +1548,52 @@
         <v>9</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="AB1" s="2" t="s">
         <v>26</v>

</xml_diff>